<commit_message>
Day 19 - steps
</commit_message>
<xml_diff>
--- a/AoC2018_19_steps.xlsx
+++ b/AoC2018_19_steps.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stefan\Programme\Python\AdventofCode2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schne\Coding\Python\Projects\AdventofCode2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14240"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="67">
   <si>
     <t>#ip 1</t>
   </si>
@@ -222,12 +222,15 @@
   </si>
   <si>
     <t>copy ip = 25 in Reg 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> …</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -308,7 +311,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -570,25 +573,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:N41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="9" width="5.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.85546875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="9" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.81640625" style="4" customWidth="1"/>
+    <col min="11" max="11" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.1796875" customWidth="1"/>
+    <col min="13" max="13" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>42</v>
       </c>
@@ -626,7 +629,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D2">
         <v>0</v>
       </c>
@@ -655,7 +658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D3">
         <v>0</v>
       </c>
@@ -687,7 +690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>0</v>
       </c>
@@ -728,7 +731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D5">
         <v>0</v>
       </c>
@@ -760,7 +763,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D6">
         <v>0</v>
       </c>
@@ -792,7 +795,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D7">
         <v>0</v>
       </c>
@@ -824,7 +827,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>0</v>
       </c>
@@ -865,7 +868,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D9">
         <v>0</v>
       </c>
@@ -897,7 +900,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D10">
         <v>0</v>
       </c>
@@ -929,7 +932,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D11">
         <v>0</v>
       </c>
@@ -961,7 +964,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1002,7 +1005,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D13">
         <v>0</v>
       </c>
@@ -1034,7 +1037,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D14">
         <v>0</v>
       </c>
@@ -1066,7 +1069,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="D15">
         <v>0</v>
       </c>
@@ -1098,7 +1101,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="5">
         <v>19</v>
       </c>
@@ -1139,7 +1142,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D17" s="5">
         <v>0</v>
       </c>
@@ -1171,7 +1174,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D18" s="5">
         <v>0</v>
       </c>
@@ -1203,7 +1206,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D19" s="5">
         <v>0</v>
       </c>
@@ -1235,7 +1238,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="5">
         <v>76</v>
       </c>
@@ -1276,7 +1279,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D21" s="5">
         <v>0</v>
       </c>
@@ -1308,7 +1311,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D22" s="5">
         <v>0</v>
       </c>
@@ -1340,7 +1343,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D23" s="5">
         <v>0</v>
       </c>
@@ -1372,7 +1375,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="5">
         <v>0</v>
       </c>
@@ -1413,7 +1416,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D25" s="5">
         <v>0</v>
       </c>
@@ -1445,7 +1448,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D26" s="5">
         <v>0</v>
       </c>
@@ -1477,7 +1480,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D27" s="5">
         <v>0</v>
       </c>
@@ -1509,7 +1512,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="5">
         <v>5</v>
       </c>
@@ -1550,7 +1553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D29" s="5">
         <v>0</v>
       </c>
@@ -1582,7 +1585,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D30" s="5">
         <v>0</v>
       </c>
@@ -1614,7 +1617,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D31" s="5">
         <v>0</v>
       </c>
@@ -1646,7 +1649,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>110</v>
       </c>
@@ -1687,7 +1690,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D33" s="5">
         <v>0</v>
       </c>
@@ -1719,7 +1722,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D34" s="5">
         <v>0</v>
       </c>
@@ -1751,7 +1754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D35" s="5">
         <v>0</v>
       </c>
@@ -1783,7 +1786,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>836</v>
       </c>
@@ -1824,7 +1827,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D37" s="5">
         <v>0</v>
       </c>
@@ -1856,7 +1859,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D38" s="5">
         <v>0</v>
       </c>
@@ -1888,7 +1891,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D39" s="5">
         <v>0</v>
       </c>
@@ -1914,7 +1917,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>25</v>
       </c>
@@ -1947,6 +1950,11 @@
       </c>
       <c r="K40" s="5" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>